<commit_message>
Save minimum speed experiment data
</commit_message>
<xml_diff>
--- a/Code/Python/Experiments/Min_speed_experiment_12-10.xlsx
+++ b/Code/Python/Experiments/Min_speed_experiment_12-10.xlsx
@@ -61,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,14 +145,14 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,49 +563,109 @@
       <c r="A23" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B23" s="0" t="n">
+        <f aca="false">235.2-50</f>
+        <v>185.2</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <f aca="false">236.4-50</f>
+        <v>186.4</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">234.3-50</f>
+        <v>184.3</v>
+      </c>
       <c r="E23" s="0" t="n">
         <f aca="false">(B23+ C23 + D23)/3</f>
-        <v>0</v>
+        <v>185.3</v>
       </c>
       <c r="F23" s="0" t="n">
         <f aca="false">E23/7</f>
-        <v>0</v>
+        <v>26.4714285714286</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">248.9-50</f>
+        <v>198.9</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <f aca="false">249.1-50</f>
+        <v>199.1</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">251.6-50</f>
+        <v>201.6</v>
+      </c>
       <c r="E24" s="0" t="n">
         <f aca="false">(B24+ C24 + D24)/3</f>
-        <v>0</v>
+        <v>199.866666666667</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">195.1-50</f>
+        <v>145.1</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <f aca="false">196.8-50</f>
+        <v>146.8</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">196.8-50</f>
+        <v>146.8</v>
+      </c>
       <c r="E25" s="0" t="n">
         <f aca="false">(B25+ C25 + D25)/3</f>
-        <v>0</v>
+        <v>146.233333333333</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">146.3-50</f>
+        <v>96.3</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <f aca="false">146.7-50</f>
+        <v>96.7</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">147.4-50</f>
+        <v>97.4</v>
+      </c>
       <c r="E26" s="0" t="n">
         <f aca="false">(B26+ C26 + D26)/3</f>
-        <v>0</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">97.1-50</f>
+        <v>47.1</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">96-50</f>
+        <v>46</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">96.5-50</f>
+        <v>46.5</v>
+      </c>
       <c r="E27" s="0" t="n">
         <f aca="false">(B27+ C27 + D27)/3</f>
-        <v>0</v>
+        <v>46.5333333333333</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,49 +692,109 @@
       <c r="A30" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">248.6-50</f>
+        <v>198.6</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">250.1-50</f>
+        <v>200.1</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">249.9-50</f>
+        <v>199.9</v>
+      </c>
       <c r="E30" s="0" t="n">
         <f aca="false">(B30+ C30 + D30)/3</f>
-        <v>0</v>
+        <v>199.533333333333</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">E30/7</f>
-        <v>0</v>
+        <v>28.5047619047619</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="B31" s="0" t="n">
+        <f aca="false">247-50</f>
+        <v>197</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <f aca="false">247.8-50</f>
+        <v>197.8</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">248.1-50</f>
+        <v>198.1</v>
+      </c>
       <c r="E31" s="0" t="n">
         <f aca="false">(B31+ C31 + D31)/3</f>
-        <v>0</v>
+        <v>197.633333333333</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="B32" s="0" t="n">
+        <f aca="false">196.4-50</f>
+        <v>146.4</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">195.9-50</f>
+        <v>145.9</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">194.9-50</f>
+        <v>144.9</v>
+      </c>
       <c r="E32" s="0" t="n">
         <f aca="false">(B32+ C32 + D32)/3</f>
-        <v>0</v>
+        <v>145.733333333333</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B33" s="0" t="n">
+        <f aca="false">145.8-50</f>
+        <v>95.8</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">146.7-50</f>
+        <v>96.7</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">146.1-50</f>
+        <v>96.1</v>
+      </c>
       <c r="E33" s="0" t="n">
         <f aca="false">(B33+ C33 + D33)/3</f>
-        <v>0</v>
+        <v>96.2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B34" s="0" t="n">
+        <f aca="false">96.3-50</f>
+        <v>46.3</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">96.4-50</f>
+        <v>46.4</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">96.2-50</f>
+        <v>46.2</v>
+      </c>
       <c r="E34" s="0" t="n">
         <f aca="false">(B34+ C34 + D34)/3</f>
-        <v>0</v>
+        <v>46.3</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,49 +821,109 @@
       <c r="A37" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B37" s="0" t="n">
+        <f aca="false">255.3-50</f>
+        <v>205.3</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <f aca="false">255.8-50</f>
+        <v>205.8</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <f aca="false">255.9-50</f>
+        <v>205.9</v>
+      </c>
       <c r="E37" s="0" t="n">
         <f aca="false">(B37+ C37 + D37)/3</f>
-        <v>0</v>
+        <v>205.666666666667</v>
       </c>
       <c r="F37" s="0" t="n">
         <f aca="false">E37/7</f>
-        <v>0</v>
+        <v>29.3809523809524</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>200</v>
       </c>
+      <c r="B38" s="0" t="n">
+        <f aca="false">251.9-50</f>
+        <v>201.9</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <f aca="false">252.2-50</f>
+        <v>202.2</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">250.5-50</f>
+        <v>200.5</v>
+      </c>
       <c r="E38" s="0" t="n">
         <f aca="false">(B38+ C38 + D38)/3</f>
-        <v>0</v>
+        <v>201.533333333333</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="B39" s="0" t="n">
+        <f aca="false">199.9-50</f>
+        <v>149.9</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">200-50</f>
+        <v>150</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">201.3-50</f>
+        <v>151.3</v>
+      </c>
       <c r="E39" s="0" t="n">
         <f aca="false">(B39+ C39 + D39)/3</f>
-        <v>0</v>
+        <v>150.4</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B40" s="0" t="n">
+        <f aca="false">149.6-50</f>
+        <v>99.6</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">149.9-50</f>
+        <v>99.9</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">150.1-50</f>
+        <v>100.1</v>
+      </c>
       <c r="E40" s="0" t="n">
         <f aca="false">(B40+ C40 + D40)/3</f>
-        <v>0</v>
+        <v>99.8666666666667</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B41" s="0" t="n">
+        <f aca="false">97.6-50</f>
+        <v>47.6</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <f aca="false">98.4-50</f>
+        <v>48.4</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <f aca="false">97.6-50</f>
+        <v>47.6</v>
+      </c>
       <c r="E41" s="0" t="n">
         <f aca="false">(B41+ C41 + D41)/3</f>
-        <v>0</v>
+        <v>47.8666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload motor frame and added 20 sec speed calibration@ 40 target
</commit_message>
<xml_diff>
--- a/Code/Python/Experiments/Min_speed_experiment_12-10.xlsx
+++ b/Code/Python/Experiments/Min_speed_experiment_12-10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t xml:space="preserve">Target = 20</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Target = 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20sec</t>
   </si>
 </sst>
 </file>
@@ -143,16 +146,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,6 +926,33 @@
       <c r="E41" s="0" t="n">
         <f aca="false">(B41+ C41 + D41)/3</f>
         <v>47.8666666666667</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>437.6</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>434.4</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>439.8</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">(B44+C44+D44)/3</f>
+        <v>437.266666666667</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <f aca="false">E44/20</f>
+        <v>21.8633333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload missing experiment data
</commit_message>
<xml_diff>
--- a/Code/Python/Experiments/Min_speed_experiment_12-10.xlsx
+++ b/Code/Python/Experiments/Min_speed_experiment_12-10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
   <si>
     <t xml:space="preserve">Target = 20</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Target = 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(LONGER TIME FOR CALIB)</t>
   </si>
   <si>
     <t xml:space="preserve">20sec</t>
@@ -146,15 +149,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,418 +545,546 @@
         <v>46.9</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>1</v>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>20.6</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">(B21+ C21 + D21)/3</f>
+        <v>20.6666666666667</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="0" t="n">
         <f aca="false">235.2-50</f>
         <v>185.2</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C24" s="0" t="n">
         <f aca="false">236.4-50</f>
         <v>186.4</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D24" s="0" t="n">
         <f aca="false">234.3-50</f>
         <v>184.3</v>
       </c>
-      <c r="E23" s="0" t="n">
-        <f aca="false">(B23+ C23 + D23)/3</f>
+      <c r="E24" s="0" t="n">
+        <f aca="false">(B24+ C24 + D24)/3</f>
         <v>185.3</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <f aca="false">E23/7</f>
+      <c r="F24" s="0" t="n">
+        <f aca="false">E24/7</f>
         <v>26.4714285714286</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B25" s="0" t="n">
         <f aca="false">248.9-50</f>
         <v>198.9</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C25" s="0" t="n">
         <f aca="false">249.1-50</f>
         <v>199.1</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D25" s="0" t="n">
         <f aca="false">251.6-50</f>
         <v>201.6</v>
       </c>
-      <c r="E24" s="0" t="n">
-        <f aca="false">(B24+ C24 + D24)/3</f>
+      <c r="E25" s="0" t="n">
+        <f aca="false">(B25+ C25 + D25)/3</f>
         <v>199.866666666667</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B26" s="0" t="n">
         <f aca="false">195.1-50</f>
         <v>145.1</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C26" s="0" t="n">
         <f aca="false">196.8-50</f>
         <v>146.8</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D26" s="0" t="n">
         <f aca="false">196.8-50</f>
         <v>146.8</v>
       </c>
-      <c r="E25" s="0" t="n">
-        <f aca="false">(B25+ C25 + D25)/3</f>
+      <c r="E26" s="0" t="n">
+        <f aca="false">(B26+ C26 + D26)/3</f>
         <v>146.233333333333</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B27" s="0" t="n">
         <f aca="false">146.3-50</f>
         <v>96.3</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C27" s="0" t="n">
         <f aca="false">146.7-50</f>
         <v>96.7</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D27" s="0" t="n">
         <f aca="false">147.4-50</f>
         <v>97.4</v>
       </c>
-      <c r="E26" s="0" t="n">
-        <f aca="false">(B26+ C26 + D26)/3</f>
+      <c r="E27" s="0" t="n">
+        <f aca="false">(B27+ C27 + D27)/3</f>
         <v>96.8</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B28" s="0" t="n">
         <f aca="false">97.1-50</f>
         <v>47.1</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C28" s="0" t="n">
         <f aca="false">96-50</f>
         <v>46</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D28" s="0" t="n">
         <f aca="false">96.5-50</f>
         <v>46.5</v>
       </c>
-      <c r="E27" s="0" t="n">
-        <f aca="false">(B27+ C27 + D27)/3</f>
+      <c r="E28" s="0" t="n">
+        <f aca="false">(B28+ C28 + D28)/3</f>
         <v>46.5333333333333</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="0" t="n">
         <f aca="false">248.6-50</f>
         <v>198.6</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C31" s="0" t="n">
         <f aca="false">250.1-50</f>
         <v>200.1</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D31" s="0" t="n">
         <f aca="false">249.9-50</f>
         <v>199.9</v>
       </c>
-      <c r="E30" s="0" t="n">
-        <f aca="false">(B30+ C30 + D30)/3</f>
+      <c r="E31" s="0" t="n">
+        <f aca="false">(B31+ C31 + D31)/3</f>
         <v>199.533333333333</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <f aca="false">E30/7</f>
+      <c r="F31" s="0" t="n">
+        <f aca="false">E31/7</f>
         <v>28.5047619047619</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B32" s="0" t="n">
         <f aca="false">247-50</f>
         <v>197</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C32" s="0" t="n">
         <f aca="false">247.8-50</f>
         <v>197.8</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D32" s="0" t="n">
         <f aca="false">248.1-50</f>
         <v>198.1</v>
       </c>
-      <c r="E31" s="0" t="n">
-        <f aca="false">(B31+ C31 + D31)/3</f>
+      <c r="E32" s="0" t="n">
+        <f aca="false">(B32+ C32 + D32)/3</f>
         <v>197.633333333333</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B33" s="0" t="n">
         <f aca="false">196.4-50</f>
         <v>146.4</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C33" s="0" t="n">
         <f aca="false">195.9-50</f>
         <v>145.9</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D33" s="0" t="n">
         <f aca="false">194.9-50</f>
         <v>144.9</v>
       </c>
-      <c r="E32" s="0" t="n">
-        <f aca="false">(B32+ C32 + D32)/3</f>
+      <c r="E33" s="0" t="n">
+        <f aca="false">(B33+ C33 + D33)/3</f>
         <v>145.733333333333</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B34" s="0" t="n">
         <f aca="false">145.8-50</f>
         <v>95.8</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C34" s="0" t="n">
         <f aca="false">146.7-50</f>
         <v>96.7</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D34" s="0" t="n">
         <f aca="false">146.1-50</f>
         <v>96.1</v>
       </c>
-      <c r="E33" s="0" t="n">
-        <f aca="false">(B33+ C33 + D33)/3</f>
+      <c r="E34" s="0" t="n">
+        <f aca="false">(B34+ C34 + D34)/3</f>
         <v>96.2</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B35" s="0" t="n">
         <f aca="false">96.3-50</f>
         <v>46.3</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C35" s="0" t="n">
         <f aca="false">96.4-50</f>
         <v>46.4</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D35" s="0" t="n">
         <f aca="false">96.2-50</f>
         <v>46.2</v>
       </c>
-      <c r="E34" s="0" t="n">
-        <f aca="false">(B34+ C34 + D34)/3</f>
+      <c r="E35" s="0" t="n">
+        <f aca="false">(B35+ C35 + D35)/3</f>
         <v>46.3</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="0" t="n">
         <f aca="false">255.3-50</f>
         <v>205.3</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C38" s="0" t="n">
         <f aca="false">255.8-50</f>
         <v>205.8</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D38" s="0" t="n">
         <f aca="false">255.9-50</f>
         <v>205.9</v>
       </c>
-      <c r="E37" s="0" t="n">
-        <f aca="false">(B37+ C37 + D37)/3</f>
+      <c r="E38" s="0" t="n">
+        <f aca="false">(B38+ C38 + D38)/3</f>
         <v>205.666666666667</v>
       </c>
-      <c r="F37" s="0" t="n">
-        <f aca="false">E37/7</f>
+      <c r="F38" s="0" t="n">
+        <f aca="false">E38/7</f>
         <v>29.3809523809524</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B39" s="0" t="n">
         <f aca="false">251.9-50</f>
         <v>201.9</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C39" s="0" t="n">
         <f aca="false">252.2-50</f>
         <v>202.2</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D39" s="0" t="n">
         <f aca="false">250.5-50</f>
         <v>200.5</v>
       </c>
-      <c r="E38" s="0" t="n">
-        <f aca="false">(B38+ C38 + D38)/3</f>
+      <c r="E39" s="0" t="n">
+        <f aca="false">(B39+ C39 + D39)/3</f>
         <v>201.533333333333</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B40" s="0" t="n">
         <f aca="false">199.9-50</f>
         <v>149.9</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C40" s="0" t="n">
         <f aca="false">200-50</f>
         <v>150</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D40" s="0" t="n">
         <f aca="false">201.3-50</f>
         <v>151.3</v>
       </c>
-      <c r="E39" s="0" t="n">
-        <f aca="false">(B39+ C39 + D39)/3</f>
+      <c r="E40" s="0" t="n">
+        <f aca="false">(B40+ C40 + D40)/3</f>
         <v>150.4</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B41" s="0" t="n">
         <f aca="false">149.6-50</f>
         <v>99.6</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C41" s="0" t="n">
         <f aca="false">149.9-50</f>
         <v>99.9</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D41" s="0" t="n">
         <f aca="false">150.1-50</f>
         <v>100.1</v>
       </c>
-      <c r="E40" s="0" t="n">
-        <f aca="false">(B40+ C40 + D40)/3</f>
+      <c r="E41" s="0" t="n">
+        <f aca="false">(B41+ C41 + D41)/3</f>
         <v>99.8666666666667</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B42" s="0" t="n">
         <f aca="false">97.6-50</f>
         <v>47.6</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C42" s="0" t="n">
         <f aca="false">98.4-50</f>
         <v>48.4</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D42" s="0" t="n">
         <f aca="false">97.6-50</f>
         <v>47.6</v>
       </c>
-      <c r="E41" s="0" t="n">
-        <f aca="false">(B41+ C41 + D41)/3</f>
+      <c r="E42" s="0" t="n">
+        <f aca="false">(B42+ C42 + D42)/3</f>
         <v>47.8666666666667</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="0" t="n">
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="0" t="n">
         <v>437.6</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C46" s="0" t="n">
         <v>434.4</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D46" s="0" t="n">
         <v>439.8</v>
       </c>
-      <c r="E44" s="0" t="n">
-        <f aca="false">(B44+C44+D44)/3</f>
+      <c r="E46" s="0" t="n">
+        <f aca="false">(B46+C46+D46)/3</f>
         <v>437.266666666667</v>
       </c>
-      <c r="F44" s="0" t="n">
-        <f aca="false">E44/20</f>
+      <c r="F46" s="0" t="n">
+        <f aca="false">E46/20</f>
         <v>21.8633333333333</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>200.2</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>198.3</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>201.1</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <f aca="false">(B47+C47+D47)/3</f>
+        <v>199.866666666667</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>149.9</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>150.9</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>149.5</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <f aca="false">(B48+C48+D48)/3</f>
+        <v>150.1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>98.7</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>98.8</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>98.9</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">(B49+C49+D49)/3</f>
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>45.1</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>46.1</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>46.4</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <f aca="false">(B50+C50+D50)/3</f>
+        <v>45.8666666666667</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <f aca="false">(B51+C51+D51)/3</f>
+        <v>23.5333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>